<commit_message>
added Figure 1 and code
</commit_message>
<xml_diff>
--- a/data/event_log_LightLamp.xlsx
+++ b/data/event_log_LightLamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zauner/Documents/Arbeit/12-TUM/Repos_Misc/SpitschanEtAl_CurrPsychiatryRep_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680750C1-6BFC-3C40-825D-9828B972A70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E6FF3F-6C83-9547-B5C2-593B1463EAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="4360" windowWidth="29040" windowHeight="15720" xr2:uid="{3AED1588-6DAE-C04F-9F05-4867B6248D8A}"/>
+    <workbookView xWindow="5520" yWindow="4360" windowWidth="29040" windowHeight="15720" xr2:uid="{3AED1588-6DAE-C04F-9F05-4867B6248D8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
   <si>
     <t>Event</t>
   </si>
@@ -62,49 +62,22 @@
     <t xml:space="preserve">start </t>
   </si>
   <si>
-    <t>baeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end </t>
-  </si>
-  <si>
-    <t>on</t>
-  </si>
-  <si>
-    <t>off</t>
-  </si>
-  <si>
     <t>therapy light</t>
   </si>
   <si>
     <t>put sweater on</t>
   </si>
   <si>
-    <t>data collection end</t>
-  </si>
-  <si>
-    <t>pre-light phase</t>
-  </si>
-  <si>
-    <t>post-light phsae</t>
-  </si>
-  <si>
-    <t>end of measurement</t>
-  </si>
-  <si>
-    <t>5541 </t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Datetime</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
-    <t>post-light phase</t>
+    <t>pre-light</t>
+  </si>
+  <si>
+    <t>post-light</t>
   </si>
 </sst>
 </file>
@@ -160,13 +133,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -501,41 +481,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB63EA0-FDD4-6247-B761-2B8980C693FF}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
     <col min="2" max="2" width="41.5" customWidth="1"/>
     <col min="3" max="4" width="25.5" customWidth="1"/>
     <col min="5" max="6" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2">
+      <c r="A2" s="5">
         <v>4789</v>
       </c>
       <c r="B2" t="s">
@@ -544,15 +523,15 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="D2" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E2" s="2">
         <v>0.40763888888888888</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>4789</v>
       </c>
       <c r="B3" t="s">
@@ -561,129 +540,135 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E3" s="2">
         <v>0.40833333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
-        <v>18</v>
+      <c r="A4" s="5">
+        <v>4789</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.40902777777777777</v>
+      <c r="D4" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.40833333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
-        <v>18</v>
+      <c r="A5" s="5">
+        <v>4789</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.44027777777777777</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5">
+        <v>4789</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.48194444444444445</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.51388888888888884</v>
+      <c r="D6" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.44027777777777777</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7">
+      <c r="A7" s="5">
         <v>4789</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.40902777777777777</v>
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.44166666666666665</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>4789</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.48194444444444445</v>
+      <c r="D8" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.44166666666666665</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
+      <c r="A9" s="5">
         <v>4789</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.51388888888888884</v>
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.44513888888888886</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
+      <c r="A10" s="5">
+        <v>4789</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.40763888888888888</v>
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.44513888888888886</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
+      <c r="A11" s="5">
+        <v>4789</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -691,146 +676,248 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="D11" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5">
+        <v>4789</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="5">
+        <v>4789</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.51388888888888884</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.40763888888888888</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E15" s="2">
         <v>0.40833333333333333</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.40833333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E17" s="2">
         <v>0.44027777777777777</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.48194444444444445</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>4789</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.44166666666666665</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>4789</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.44513888888888886</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D18" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.44027777777777777</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B20" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="D20" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E21" s="2">
         <v>0.48680555555555555</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.48680555555555555</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.48749999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E17" s="3">
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E24" s="2">
         <v>0.48749999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>4789</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.51388888888888884</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="5">
-        <v>45960</v>
-      </c>
-      <c r="E19" s="3">
+    <row r="25" spans="1:5">
+      <c r="A25" s="6">
+        <v>5541</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>45960</v>
+      </c>
+      <c r="E25" s="2">
         <v>0.51388888888888884</v>
       </c>
     </row>

</xml_diff>